<commit_message>
saving excel file to repo
</commit_message>
<xml_diff>
--- a/resources/2021/day-24-monad.xlsx
+++ b/resources/2021/day-24-monad.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wevrem/Documents/programming/clojure/advent-of-code/resources/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F00A2F-EF35-7240-A9C8-E152B962B389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E975B4-F072-4846-8DB6-41784E06E8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-7220" windowWidth="33480" windowHeight="21180" activeTab="1" xr2:uid="{A4125FCF-FD30-1B48-9536-1BDB68B83904}"/>
+    <workbookView xWindow="47660" yWindow="-7460" windowWidth="42660" windowHeight="22140" activeTab="1" xr2:uid="{A4125FCF-FD30-1B48-9536-1BDB68B83904}"/>
   </bookViews>
   <sheets>
     <sheet name="smallest" sheetId="1" r:id="rId1"/>
     <sheet name="largest" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>digit</t>
   </si>
@@ -78,12 +78,24 @@
   <si>
     <t>d</t>
   </si>
+  <si>
+    <t>&lt;-- These are like brackets: 1's are opening parens and 26's are closing parens, and they form nested pairs</t>
+  </si>
+  <si>
+    <t>&lt;-- For a pair, the opening C parameter, and closing B parameter determine the valid range of digits</t>
+  </si>
+  <si>
+    <t>&lt;-- C_start + B_end determine the valid range of digits</t>
+  </si>
+  <si>
+    <t>&lt;-- The yellow and orange digits are fixed, they have to be a specific value in order to trigger the division and reduce z</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +106,13 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,21 +255,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -845,55 +857,55 @@
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <f>C9</f>
+        <f t="shared" ref="D8:P8" si="0">C9</f>
         <v>13</v>
       </c>
       <c r="E8" s="1">
-        <f>D9</f>
+        <f t="shared" si="0"/>
         <v>346</v>
       </c>
       <c r="F8" s="1">
-        <f>E9</f>
+        <f t="shared" si="0"/>
         <v>9005</v>
       </c>
       <c r="G8" s="1">
-        <f>F9</f>
+        <f t="shared" si="0"/>
         <v>234136</v>
       </c>
       <c r="H8" s="1">
-        <f>G9</f>
+        <f t="shared" si="0"/>
         <v>9005</v>
       </c>
       <c r="I8" s="1">
-        <f>H9</f>
+        <f t="shared" si="0"/>
         <v>234147</v>
       </c>
       <c r="J8" s="1">
-        <f>I9</f>
+        <f t="shared" si="0"/>
         <v>6087836</v>
       </c>
       <c r="K8" s="1">
-        <f>J9</f>
+        <f t="shared" si="0"/>
         <v>234147</v>
       </c>
       <c r="L8" s="1">
-        <f>K9</f>
+        <f t="shared" si="0"/>
         <v>9005</v>
       </c>
       <c r="M8" s="1">
-        <f>L9</f>
+        <f t="shared" si="0"/>
         <v>346</v>
       </c>
       <c r="N8" s="1">
-        <f>M9</f>
+        <f t="shared" si="0"/>
         <v>9005</v>
       </c>
       <c r="O8" s="1">
-        <f>N9</f>
+        <f t="shared" si="0"/>
         <v>346</v>
       </c>
       <c r="P8" s="1">
-        <f>O9</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
@@ -906,55 +918,55 @@
         <v>13</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" ref="D9:P9" si="0">_xlfn.LET(_xlpm.Z,D8,_xlpm.A,D4,_xlpm.B,D5,_xlpm.C,D6,_xlpm.dig,D7,IF((_xlpm.B+MOD(_xlpm.Z,26))=_xlpm.dig,INT(_xlpm.Z/_xlpm.A),INT(_xlpm.Z/_xlpm.A)*26+_xlpm.dig+_xlpm.C))</f>
+        <f t="shared" ref="D9:P9" si="1">_xlfn.LET(_xlpm.Z,D8,_xlpm.A,D4,_xlpm.B,D5,_xlpm.C,D6,_xlpm.dig,D7,IF((_xlpm.B+MOD(_xlpm.Z,26))=_xlpm.dig,INT(_xlpm.Z/_xlpm.A),INT(_xlpm.Z/_xlpm.A)*26+_xlpm.dig+_xlpm.C))</f>
         <v>346</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9005</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>234136</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9005</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>234147</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6087836</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>234147</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9005</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>346</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9005</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>346</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -967,55 +979,55 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:P11" si="1">MOD(D8,26)</f>
+        <f t="shared" ref="D11:P11" si="2">MOD(D8,26)</f>
         <v>13</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="P11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
     </row>
@@ -1028,55 +1040,55 @@
         <v>14</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="D12:P12" si="2">D11+D5</f>
+        <f t="shared" ref="D12:P12" si="3">D11+D5</f>
         <v>28</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="N12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="P12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
@@ -1089,55 +1101,55 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="D13:P13" si="3">INT(D8/D4)</f>
+        <f t="shared" ref="D13:P13" si="4">INT(D8/D4)</f>
         <v>13</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>346</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9005</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9005</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9005</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>234147</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>234147</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9005</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>346</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>346</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>346</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="P13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1146,59 +1158,59 @@
         <v>8</v>
       </c>
       <c r="C14" s="1">
-        <f>INT(C8/C4)*26+C7+C6</f>
+        <f t="shared" ref="C14:P14" si="5">INT(C8/C4)*26+C7+C6</f>
         <v>13</v>
       </c>
       <c r="D14" s="1">
-        <f>INT(D8/D4)*26+D7+D6</f>
+        <f t="shared" si="5"/>
         <v>346</v>
       </c>
       <c r="E14" s="1">
-        <f>INT(E8/E4)*26+E7+E6</f>
+        <f t="shared" si="5"/>
         <v>9005</v>
       </c>
       <c r="F14" s="1">
-        <f>INT(F8/F4)*26+F7+F6</f>
+        <f t="shared" si="5"/>
         <v>234136</v>
       </c>
       <c r="G14" s="1">
-        <f>INT(G8/G4)*26+G7+G6</f>
+        <f t="shared" si="5"/>
         <v>234135</v>
       </c>
       <c r="H14" s="1">
-        <f>INT(H8/H4)*26+H7+H6</f>
+        <f t="shared" si="5"/>
         <v>234147</v>
       </c>
       <c r="I14" s="1">
-        <f>INT(I8/I4)*26+I7+I6</f>
+        <f t="shared" si="5"/>
         <v>6087836</v>
       </c>
       <c r="J14" s="1">
-        <f>INT(J8/J4)*26+J7+J6</f>
+        <f t="shared" si="5"/>
         <v>6087828</v>
       </c>
       <c r="K14" s="1">
-        <f>INT(K8/K4)*26+K7+K6</f>
+        <f t="shared" si="5"/>
         <v>234134</v>
       </c>
       <c r="L14" s="1">
-        <f>INT(L8/L4)*26+L7+L6</f>
+        <f t="shared" si="5"/>
         <v>9006</v>
       </c>
       <c r="M14" s="1">
-        <f>INT(M8/M4)*26+M7+M6</f>
+        <f t="shared" si="5"/>
         <v>9005</v>
       </c>
       <c r="N14" s="1">
-        <f>INT(N8/N4)*26+N7+N6</f>
+        <f t="shared" si="5"/>
         <v>9000</v>
       </c>
       <c r="O14" s="1">
-        <f>INT(O8/O4)*26+O7+O6</f>
+        <f t="shared" si="5"/>
         <v>349</v>
       </c>
       <c r="P14" s="1">
-        <f>INT(P8/P4)*26+P7+P6</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -1349,7 +1361,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G7 J7:L7 N7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>G7&lt;&gt;G12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1359,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D980EAC-FCCF-5F4F-AA60-0228A883A9FA}">
-  <dimension ref="A3:P24"/>
+  <dimension ref="A3:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.2"/>
@@ -1373,7 +1385,7 @@
     <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1420,7 +1432,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1466,8 +1478,11 @@
       <c r="P4" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q4" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1513,8 +1528,11 @@
       <c r="P5" s="1">
         <v>-4</v>
       </c>
-    </row>
-    <row r="6" spans="2:16" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1561,7 +1579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1614,8 +1632,11 @@
         <f>P12</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1623,59 +1644,59 @@
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <f>C9</f>
+        <f t="shared" ref="D8:P8" si="0">C9</f>
         <v>13</v>
       </c>
       <c r="E8" s="1">
-        <f>D9</f>
+        <f t="shared" si="0"/>
         <v>347</v>
       </c>
       <c r="F8" s="1">
-        <f>E9</f>
+        <f t="shared" si="0"/>
         <v>9032</v>
       </c>
       <c r="G8" s="1">
-        <f>F9</f>
+        <f t="shared" si="0"/>
         <v>234843</v>
       </c>
       <c r="H8" s="1">
-        <f>G9</f>
+        <f t="shared" si="0"/>
         <v>9032</v>
       </c>
       <c r="I8" s="1">
-        <f>H9</f>
+        <f t="shared" si="0"/>
         <v>234856</v>
       </c>
       <c r="J8" s="1">
-        <f>I9</f>
+        <f t="shared" si="0"/>
         <v>6106276</v>
       </c>
       <c r="K8" s="1">
-        <f>J9</f>
+        <f t="shared" si="0"/>
         <v>234856</v>
       </c>
       <c r="L8" s="1">
-        <f>K9</f>
+        <f t="shared" si="0"/>
         <v>9032</v>
       </c>
       <c r="M8" s="1">
-        <f>L9</f>
+        <f t="shared" si="0"/>
         <v>347</v>
       </c>
       <c r="N8" s="1">
-        <f>M9</f>
+        <f t="shared" si="0"/>
         <v>9033</v>
       </c>
       <c r="O8" s="1">
-        <f>N9</f>
+        <f t="shared" si="0"/>
         <v>347</v>
       </c>
       <c r="P8" s="1">
-        <f>O9</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1684,59 +1705,59 @@
         <v>13</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" ref="D9:P9" si="0">_xlfn.LET(_xlpm.Z,D8,_xlpm.A,D4,_xlpm.B,D5,_xlpm.C,D6,_xlpm.dig,D7,IF((_xlpm.B+MOD(_xlpm.Z,26))=_xlpm.dig,INT(_xlpm.Z/_xlpm.A),INT(_xlpm.Z/_xlpm.A)*26+_xlpm.dig+_xlpm.C))</f>
+        <f t="shared" ref="D9:P9" si="1">_xlfn.LET(_xlpm.Z,D8,_xlpm.A,D4,_xlpm.B,D5,_xlpm.C,D6,_xlpm.dig,D7,IF((_xlpm.B+MOD(_xlpm.Z,26))=_xlpm.dig,INT(_xlpm.Z/_xlpm.A),INT(_xlpm.Z/_xlpm.A)*26+_xlpm.dig+_xlpm.C))</f>
         <v>347</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9032</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>234843</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9032</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>234856</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6106276</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>234856</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9032</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>347</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9033</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>347</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1745,59 +1766,59 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:P11" si="1">MOD(D8,26)</f>
+        <f t="shared" ref="D11:P11" si="2">MOD(D8,26)</f>
         <v>13</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="P11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1806,59 +1827,59 @@
         <v>14</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="D12:P12" si="2">D11+D5</f>
+        <f t="shared" ref="D12:P12" si="3">D11+D5</f>
         <v>28</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="N12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="P12" s="1">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1867,126 +1888,126 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="D13:P13" si="3">INT(D8/D4)</f>
+        <f t="shared" ref="D13:P13" si="4">INT(D8/D4)</f>
         <v>13</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>347</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9032</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9032</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9032</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>234856</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>234856</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9032</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>347</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>347</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>347</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="P13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1">
-        <f>INT(C8/C4)*26+C7+C6</f>
+        <f t="shared" ref="C14:P14" si="5">INT(C8/C4)*26+C7+C6</f>
         <v>13</v>
       </c>
       <c r="D14" s="1">
-        <f>INT(D8/D4)*26+D7+D6</f>
+        <f t="shared" si="5"/>
         <v>347</v>
       </c>
       <c r="E14" s="1">
-        <f>INT(E8/E4)*26+E7+E6</f>
+        <f t="shared" si="5"/>
         <v>9032</v>
       </c>
       <c r="F14" s="1">
-        <f>INT(F8/F4)*26+F7+F6</f>
+        <f t="shared" si="5"/>
         <v>234843</v>
       </c>
       <c r="G14" s="1">
-        <f>INT(G8/G4)*26+G7+G6</f>
+        <f t="shared" si="5"/>
         <v>234842</v>
       </c>
       <c r="H14" s="1">
-        <f>INT(H8/H4)*26+H7+H6</f>
+        <f t="shared" si="5"/>
         <v>234856</v>
       </c>
       <c r="I14" s="1">
-        <f>INT(I8/I4)*26+I7+I6</f>
+        <f t="shared" si="5"/>
         <v>6106276</v>
       </c>
       <c r="J14" s="1">
-        <f>INT(J8/J4)*26+J7+J6</f>
+        <f t="shared" si="5"/>
         <v>6106268</v>
       </c>
       <c r="K14" s="1">
-        <f>INT(K8/K4)*26+K7+K6</f>
+        <f t="shared" si="5"/>
         <v>234843</v>
       </c>
       <c r="L14" s="1">
-        <f>INT(L8/L4)*26+L7+L6</f>
+        <f t="shared" si="5"/>
         <v>9033</v>
       </c>
       <c r="M14" s="1">
-        <f>INT(M8/M4)*26+M7+M6</f>
+        <f t="shared" si="5"/>
         <v>9033</v>
       </c>
       <c r="N14" s="1">
-        <f>INT(N8/N4)*26+N7+N6</f>
+        <f t="shared" si="5"/>
         <v>9028</v>
       </c>
       <c r="O14" s="1">
-        <f>INT(O8/O4)*26+O7+O6</f>
+        <f t="shared" si="5"/>
         <v>350</v>
       </c>
       <c r="P14" s="1">
-        <f>INT(P8/P4)*26+P7+P6</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="9"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E18" s="9"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -1996,7 +2017,7 @@
       <c r="K18" s="10"/>
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -2010,7 +2031,7 @@
       <c r="N19" s="10"/>
       <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -2026,7 +2047,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="9"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
@@ -2059,7 +2080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2092,7 +2113,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
@@ -2124,10 +2145,13 @@
         <f>M6+N5</f>
         <v>-6</v>
       </c>
+      <c r="Q24" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G7 J7:L7 N7">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>G7&lt;&gt;G12</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>